<commit_message>
Completed currency forward contract model
</commit_message>
<xml_diff>
--- a/financial_derivates_futures_options/forwards.xlsx
+++ b/financial_derivates_futures_options/forwards.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_derivates/financial_derivates_futures_options/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C559025-EF59-E447-8985-B26256DE7BF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01C8307-785E-C143-8847-CE684E57461E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{3E6DBD08-5F34-6444-93B2-5BE496AD5604}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{3E6DBD08-5F34-6444-93B2-5BE496AD5604}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cotton Forward" sheetId="1" r:id="rId1"/>
+    <sheet name="USD-RS Forward" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">'USD-RS Forward'!$B$22:$B$25</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'USD-RS Forward'!$F$22:$F$25</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Forwards</t>
   </si>
@@ -34,9 +39,6 @@
   </si>
   <si>
     <t xml:space="preserve">The current price (01-Dec-2020) of cotton is </t>
-  </si>
-  <si>
-    <t>Rs 19750</t>
   </si>
   <si>
     <t>per Bale (per 170 kg)</t>
@@ -86,6 +88,105 @@
   </si>
   <si>
     <t>Speculator's Payoff</t>
+  </si>
+  <si>
+    <t>Draw Hedger's Pay off on a graph</t>
+  </si>
+  <si>
+    <t>Current exchange rate</t>
+  </si>
+  <si>
+    <t>Rs/USD</t>
+  </si>
+  <si>
+    <t>I have imported goods and have to pay</t>
+  </si>
+  <si>
+    <t>after 3 months in dollars</t>
+  </si>
+  <si>
+    <t>If Rs/USD becomes higher than</t>
+  </si>
+  <si>
+    <t>Rs Depreciates / Dollar Appreciates</t>
+  </si>
+  <si>
+    <t>If RS/USD becomes lower than</t>
+  </si>
+  <si>
+    <t>RS Appreciates / Dollars Depreciates</t>
+  </si>
+  <si>
+    <t>Thus business is exposed to fluctuation in currency 
+rate 2 months forward in USD is going at Rs 77</t>
+  </si>
+  <si>
+    <t>SHOW</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- How do I use Forwards to hedge my risk?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- show Hedger's &amp; Speculator's Payoffs of Forward
+hedge if the USD price after 3 months is Rs 70, 72, 80,
+85, assuming Cash Settlement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Plot a graph showing Payoff for Hedger and Speculator</t>
+    </r>
+  </si>
+  <si>
+    <t>A - I take a Long position in USD Forwards</t>
+  </si>
+  <si>
+    <t>Spot Price (Market Price after 3 months)</t>
+  </si>
+  <si>
+    <t>Strike Price</t>
+  </si>
+  <si>
+    <t>Buying from Market at</t>
   </si>
 </sst>
 </file>
@@ -236,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -247,6 +348,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -259,10 +364,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,6 +385,2075 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Payoffs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cotton Forward'!$B$29:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cotton Forward'!$C$29:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2880</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1880</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0FAD-0F46-9C3A-23F6FECB20A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Cotton Forward'!$B$29:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cotton Forward'!$E$29:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>19880</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19880</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19880</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19880</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19880</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19880</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0FAD-0F46-9C3A-23F6FECB20A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2037043311"/>
+        <c:axId val="2037044959"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2037043311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2037044959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2037044959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2037043311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>PayOff</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'USD-RS Forward'!$F$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hedger's Payoff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'USD-RS Forward'!$B$22:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'USD-RS Forward'!$F$22:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F759-CC4D-8F65-83BC321C0C63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'USD-RS Forward'!$D$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speculator's Payoff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'USD-RS Forward'!$B$22:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'USD-RS Forward'!$D$22:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F759-CC4D-8F65-83BC321C0C63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1906611711"/>
+        <c:axId val="1907327487"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1906611711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1907327487"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1907327487"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1906611711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3587750</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E116217-33D5-3042-A879-2B7B5394373E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFBD899C-66A3-C04D-989E-F31FEEBBDF09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,10 +2753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CCC5F0-82A8-D642-9CAE-F07F67DB712C}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,17 +2783,17 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1">
+        <v>19750</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -625,18 +2801,18 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>19880</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -644,12 +2820,12 @@
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -657,21 +2833,21 @@
         <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -738,31 +2914,31 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="10"/>
-      <c r="C24" s="11" t="s">
-        <v>17</v>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+      <c r="B27" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="D28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
@@ -829,7 +3005,7 @@
         <v>19880</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="4">
         <v>20000</v>
       </c>
@@ -845,7 +3021,7 @@
         <v>19880</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" s="4">
         <v>21000</v>
       </c>
@@ -861,7 +3037,7 @@
         <v>19880</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="4">
         <v>22000</v>
       </c>
@@ -877,12 +3053,20 @@
         <v>19880</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C36" s="11" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>4</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -891,5 +3075,233 @@
     <mergeCell ref="B27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A980822F-18CA-194B-A225-755BBF9DDAEC}">
+  <dimension ref="B1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <f>D1</f>
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <f>D1</f>
+        <v>75</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="B14" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="2:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="4">
+        <v>70</v>
+      </c>
+      <c r="C22" s="4">
+        <v>77</v>
+      </c>
+      <c r="D22" s="4">
+        <f>B22-C22</f>
+        <v>-7</v>
+      </c>
+      <c r="E22" s="4">
+        <f>-1*B22</f>
+        <v>-70</v>
+      </c>
+      <c r="F22" s="4">
+        <f>E22+D22</f>
+        <v>-77</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="4">
+        <v>72</v>
+      </c>
+      <c r="C23" s="4">
+        <v>77</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" ref="D23:D25" si="0">B23-C23</f>
+        <v>-5</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" ref="E23:E25" si="1">-1*B23</f>
+        <v>-72</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" ref="F23:F25" si="2">E23+D23</f>
+        <v>-77</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="4">
+        <v>80</v>
+      </c>
+      <c r="C24" s="4">
+        <v>77</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="1"/>
+        <v>-80</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="2"/>
+        <v>-77</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="4">
+        <v>85</v>
+      </c>
+      <c r="C25" s="4">
+        <v>77</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="1"/>
+        <v>-85</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="2"/>
+        <v>-77</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B20:F20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed equity forward contract model
</commit_message>
<xml_diff>
--- a/financial_derivates_futures_options/forwards.xlsx
+++ b/financial_derivates_futures_options/forwards.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_derivates/financial_derivates_futures_options/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01C8307-785E-C143-8847-CE684E57461E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD42EFC-BF08-B34F-B726-4F043AECC6DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{3E6DBD08-5F34-6444-93B2-5BE496AD5604}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="2" xr2:uid="{3E6DBD08-5F34-6444-93B2-5BE496AD5604}"/>
   </bookViews>
   <sheets>
     <sheet name="Cotton Forward" sheetId="1" r:id="rId1"/>
     <sheet name="USD-RS Forward" sheetId="2" r:id="rId2"/>
+    <sheet name="Equity Forward" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">'USD-RS Forward'!$B$22:$B$25</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'USD-RS Forward'!$F$22:$F$25</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'Equity Forward'!$B$29:$B$32</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Equity Forward'!$F$29:$F$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>Forwards</t>
   </si>
@@ -187,6 +188,105 @@
   </si>
   <si>
     <t>Buying from Market at</t>
+  </si>
+  <si>
+    <t>Today is 1st Dec 2020</t>
+  </si>
+  <si>
+    <t>RIL shares are currently quoted at</t>
+  </si>
+  <si>
+    <t>I want to buy shares of Reliance Industries Ltd (RIL)</t>
+  </si>
+  <si>
+    <t>But cannot but today as don’t hace enough money to invest</t>
+  </si>
+  <si>
+    <t>However I will get my Fixed Deposit of Rs 50,000 getting matured</t>
+  </si>
+  <si>
+    <t>per share</t>
+  </si>
+  <si>
+    <t>in Jan 2021</t>
+  </si>
+  <si>
+    <t>I plan to invest that money in shares of RIL</t>
+  </si>
+  <si>
+    <t>Jan Forward of RIL is going at Rs 1968</t>
+  </si>
+  <si>
+    <t>I fear the prices of RIL shares will go up</t>
+  </si>
+  <si>
+    <t>if prices go down, I am happy</t>
+  </si>
+  <si>
+    <t>But if prices go up, I am unhappy</t>
+  </si>
+  <si>
+    <t>What do I do?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHOW </t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- How do I use Forwards to hedge my risk? What position will I 
+take in Forwards?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Show Hedgers's &amp; Speculator's Payoffs for Forwards hedge if 
+prices in Jan 2021 are 1600, 1800,2000,2200, assuming cash 
+settlement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- plot a graph showing Payoff for Hedger and Speculator</t>
+    </r>
+  </si>
+  <si>
+    <t>Spot Price (Jan 2021)</t>
+  </si>
+  <si>
+    <t>I will buy a forward contract</t>
   </si>
 </sst>
 </file>
@@ -352,6 +452,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -363,12 +469,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,6 +1375,435 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Payoff</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Equity Forward'!$F$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hedger's Payoff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Equity Forward'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Equity Forward'!$F$29:$F$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-1968</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1968</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1968</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59A6-5644-A510-64E7484EEBD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Equity Forward'!$D$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speculator's Payoff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Equity Forward'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Equity Forward'!$D$29:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-368</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>232</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-59A6-5644-A510-64E7484EEBD2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2068336399"/>
+        <c:axId val="2068360255"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2068336399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2068360255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2068360255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2068336399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1355,6 +1884,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1859,6 +2428,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2436,6 +3521,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFBD899C-66A3-C04D-989E-F31FEEBBDF09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C42E71C-7927-8043-BA09-A31F69245BBA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2755,8 +3881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CCC5F0-82A8-D642-9CAE-F07F67DB712C}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:E36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2837,10 +3963,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="11"/>
     </row>
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
@@ -2920,12 +4046,12 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
@@ -3083,8 +4209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A980822F-18CA-194B-A225-755BBF9DDAEC}">
   <dimension ref="B1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3141,7 +4267,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="1">
@@ -3159,7 +4285,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3179,13 +4305,13 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="2:6" ht="68" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
@@ -3304,4 +4430,279 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B855416-8C5D-0545-B999-1DAD655B53BE}">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1954</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="4">
+        <v>1600</v>
+      </c>
+      <c r="C29" s="4">
+        <f>$C$7</f>
+        <v>1968</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" ref="D29:D31" si="0">B29-C29</f>
+        <v>-368</v>
+      </c>
+      <c r="E29" s="4">
+        <v>-1600</v>
+      </c>
+      <c r="F29" s="4">
+        <f>E29+D29</f>
+        <v>-1968</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="4">
+        <v>1800</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" ref="C30:C32" si="1">$C$7</f>
+        <v>1968</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="0"/>
+        <v>-168</v>
+      </c>
+      <c r="E30" s="4">
+        <v>-1800</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" ref="F30:F32" si="2">E30+D30</f>
+        <v>-1968</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="4">
+        <v>2000</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="1"/>
+        <v>1968</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E31" s="4">
+        <v>-2000</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="2"/>
+        <v>-1968</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="4">
+        <v>2200</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="1"/>
+        <v>1968</v>
+      </c>
+      <c r="D32" s="4">
+        <f>B32-C32</f>
+        <v>232</v>
+      </c>
+      <c r="E32" s="4">
+        <v>-2200</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="2"/>
+        <v>-1968</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B27:F27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>